<commit_message>
Updates of scriptKeywords file
</commit_message>
<xml_diff>
--- a/docs/scriptKeywords.xlsx
+++ b/docs/scriptKeywords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewProgramStructure\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roh\Documents\python\Opt_test\NewTest\Optimus\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5F1F20-0734-47E0-B19B-2CD0CF52068A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0819D760-0DC9-4B4C-B1D9-7FDD0318F7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="200">
   <si>
     <t>   # ------------------ code processing functions ------------------------------</t>
   </si>
@@ -421,6 +421,219 @@
   </si>
   <si>
     <t>runModule:iCristal2</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Does not update templated values</t>
+  </si>
+  <si>
+    <t>Updates templated values and prints to console / log</t>
+  </si>
+  <si>
+    <t>Updates templated values and logs result</t>
+  </si>
+  <si>
+    <t>Statement</t>
+  </si>
+  <si>
+    <t>raiseError:</t>
+  </si>
+  <si>
+    <t>Raise error</t>
+  </si>
+  <si>
+    <t>code value</t>
+  </si>
+  <si>
+    <t>raiseError:&lt;iterationCount&gt;</t>
+  </si>
+  <si>
+    <t>Raises error and returns code value in log</t>
+  </si>
+  <si>
+    <t>strPattern, strSearch, variable_name</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>strPattern = regex pattern to search
+strSearch = string to search.  Can be a templated value
+variable_name = saves result to a variable which can be accessed as a templated value e.g. &lt;variable_name&gt;</t>
+  </si>
+  <si>
+    <t>    # ------------------ Concepts ------------------------------</t>
+  </si>
+  <si>
+    <t>TEMPLATED VALUES</t>
+  </si>
+  <si>
+    <t>runJupyterNb:</t>
+  </si>
+  <si>
+    <t>User defined routines</t>
+  </si>
+  <si>
+    <t>iterationCount:</t>
+  </si>
+  <si>
+    <t>DFcreate:</t>
+  </si>
+  <si>
+    <t>makeDir:</t>
+  </si>
+  <si>
+    <t>removeFile:</t>
+  </si>
+  <si>
+    <t>runInBackground:</t>
+  </si>
+  <si>
+    <t>increment:</t>
+  </si>
+  <si>
+    <t>urlcontains:</t>
+  </si>
+  <si>
+    <t>present:</t>
+  </si>
+  <si>
+    <t>exist:</t>
+  </si>
+  <si>
+    <t>count:</t>
+  </si>
+  <si>
+    <t>type:</t>
+  </si>
+  <si>
+    <t>telegram:</t>
+  </si>
+  <si>
+    <t>email:</t>
+  </si>
+  <si>
+    <t>waitEmailComplete:</t>
+  </si>
+  <si>
+    <t>MODULES</t>
+  </si>
+  <si>
+    <t>A Module in OPTIMUS is basically a worksheet containing all automation steps to be executed.</t>
+  </si>
+  <si>
+    <t>Run step</t>
+  </si>
+  <si>
+    <t>A step in a Module can call steps in another worksheet/Module using the runModule keyword command.
+Modules can be used to organize logical groups of automation steps e.g. for application logon.  It promotes reuse of scripts.</t>
+  </si>
+  <si>
+    <t>Each execution step in the module automation script is defined with a Type, Object, Key, Value and Comments.</t>
+  </si>
+  <si>
+    <t>Keywords:parameter(s)</t>
+  </si>
+  <si>
+    <t>The headers - Type, Object are case sensitive.  But can be in any order.</t>
+  </si>
+  <si>
+    <t>For list objects, this is usually a Keyword command to be executed by Optimus.
+For key objects, this will be the label of a key value pair.  E.g. saveFolderPath is the key label, and the value will contain the path name.</t>
+  </si>
+  <si>
+    <t>Comments are purely for user documentation of steps. It is not processed by optimus.</t>
+  </si>
+  <si>
+    <t>Key and Value</t>
+  </si>
+  <si>
+    <t>if:&lt;URL_Dclick_Pages:CropImage&gt;:cropFiles</t>
+  </si>
+  <si>
+    <t>Any run step can be defined with "templated values" which will be updated with the actual value when the step is processed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A TEMPLATED VALUE to be updated in a run step command is defined with the "&lt; &gt;" or "{{ }}" brackets.  Within the special &lt;&gt; or {{}} bracket, you define the name of the object which will be updated by optimus with the value of that "key" or "table" object.  "table" object is additionally defined with the object name and column or field name like "&lt;table_name:column_name&gt;"  </t>
+  </si>
+  <si>
+    <t>If the condition evaluates to be true, the defined list object containing some automation steps is run</t>
+  </si>
+  <si>
+    <t>Refer to the "concepts" section about "list" objects, which are logical blocks of automation steps</t>
+  </si>
+  <si>
+    <t>Refer to the "concepts" section about "modules", which are higher levels of logical groups of automation steps compared to list objects.</t>
+  </si>
+  <si>
+    <t>Type and Object</t>
+  </si>
+  <si>
+    <t>Keyword commards must have a semi-colon. And additional parameters (from zero to many input parameters) may be provided after the semi-colon.  Keywords are not case sensitive.</t>
+  </si>
+  <si>
+    <t>Type defines the type of Object in the script.  Can be a list, key, or table object type.
+And every Object is given a name in the Object column.  The Object names are case sensitive and must match exactly when referenced from other parts of the script.</t>
+  </si>
+  <si>
+    <t>"list" are a collection or block of run steps.  The name of the list object is like a Keyword for a user defined list of automation steps, that can be referenced from other parts of the script.  This list "Keyword" is case sensitive.
+"key" can be one or more key and value pairs of objects used by the automation script to update templated values.  When named as "constants" or "variables" in the Object column - they indicate special type of key value pairs used by the script.  "key" object can also have multiple key value records/rows.
+"table" is a special 2 dimensional object with multiple columns (field names).  They are like "key" object - but with more than one column or user defined column names.  The first row of the table object is the column header names.  
+Both "key" and "table" objects are iterable.  i.e. they can be executed with a iterate keyword to loop through each record row for processing.</t>
+  </si>
+  <si>
+    <t>email:Email_Lists</t>
+  </si>
+  <si>
+    <t>Wait for all emails in outbox sent folder to be sent before proceeding to next step.</t>
+  </si>
+  <si>
+    <t>Used in conjunction with email command.  If not used, the automation script may end after email step, with some mails still unsent out from the outbox folder.</t>
+  </si>
+  <si>
+    <t>Sends an email via outlook</t>
+  </si>
+  <si>
+    <t>Sends a telegram message</t>
+  </si>
+  <si>
+    <t>Type into a selector input box</t>
+  </si>
+  <si>
+    <t>Checks if selector exist</t>
+  </si>
+  <si>
+    <t>Checks if selector is present</t>
+  </si>
+  <si>
+    <t>Sets a value in a variable</t>
+  </si>
+  <si>
+    <t>Create a directory</t>
+  </si>
+  <si>
+    <t>Removes a file</t>
+  </si>
+  <si>
+    <t>Renames a recently downloaded file to a given name</t>
+  </si>
+  <si>
+    <t>Used when the website does not allow you to specify a name for the download file and the download file has a random generated name</t>
+  </si>
+  <si>
+    <t>Run a jupyter notebook with parameters</t>
+  </si>
+  <si>
+    <t>Works with a table object or a json parameter.  The table object or json parameter must contain data with the following labels ['To', 'CC', 'Subject', 'Body', 'HTMLBody', 'Attachment', 'boolDisplay', 'boolRun', 'boolForce'].
+boolDisplay - displays email message instead of sending if TRUE.  Useful for testing.  boolRun - sends the email if TRUE.  Useful to set conditions for emailing.  boolForce - will overwrite the boolRun condition if TRUE.</t>
   </si>
 </sst>
 </file>
@@ -464,12 +677,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,21 +966,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="B61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="3" width="44.42578125" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="52.28515625" customWidth="1"/>
+    <col min="7" max="7" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -775,15 +993,24 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -793,30 +1020,48 @@
       <c r="C4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>92</v>
       </c>
       <c r="B6" t="s">
         <v>94</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -824,443 +1069,684 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>82</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>91</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>90</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E10" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>79</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>107</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>130</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E11" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>97</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+    <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>78</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>102</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>101</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>77</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>117</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>110</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>76</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>116</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>115</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F22" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>112</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>113</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F23" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>74</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>73</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>118</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>71</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>119</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>70</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>120</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>22</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>21</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>65</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>64</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="37" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>41</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B40" t="s">
         <v>40</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C40" t="s">
         <v>42</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>48</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>47</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="43" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>46</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B45" t="s">
+        <v>196</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E45" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F45" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="48" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>50</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B50" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>14</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B51" t="s">
         <v>15</v>
       </c>
-      <c r="D44" t="s">
+      <c r="F51" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B52" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>54</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B53" t="s">
         <v>103</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C53" t="s">
         <v>53</v>
       </c>
-      <c r="D46" t="s">
+      <c r="F53" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>55</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B54" t="s">
         <v>105</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C54" t="s">
         <v>104</v>
       </c>
-      <c r="D47" t="s">
+      <c r="F54" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>57</v>
       </c>
-      <c r="C48" t="s">
+      <c r="B55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="56" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>59</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B58" t="s">
         <v>58</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C58" t="s">
         <v>85</v>
       </c>
-      <c r="D49" t="s">
+      <c r="F58" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>9</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B59" t="s">
         <v>8</v>
       </c>
-      <c r="D50" t="s">
+      <c r="F59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="60" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>61</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B63" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="64" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>19</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B65" t="s">
         <v>87</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C65" t="s">
         <v>88</v>
       </c>
-      <c r="D52" t="s">
+      <c r="F65" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="66" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="4" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>18</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B69" t="s">
         <v>17</v>
       </c>
-      <c r="D53" t="s">
+      <c r="F69" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="4" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:6" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>148</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F78" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D44" r:id="rId1" display="url:URL_Dclick_Pages" xr:uid="{5674B4B1-67B6-453C-8E59-538F39EE576D}"/>
+    <hyperlink ref="F51" r:id="rId1" display="url:URL_Dclick_Pages" xr:uid="{5674B4B1-67B6-453C-8E59-538F39EE576D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1494,9 +1980,28 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C081DC7-6F6E-403C-87DE-243AB83C04CD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C081DC7-6F6E-403C-87DE-243AB83C04CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9acd4cc3-1974-45d5-bfd4-2e52d38b09ac"/>
+    <ds:schemaRef ds:uri="f684fbb7-43f1-4b17-9ab1-c03d5e423760"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CB9A2C0-E860-4BCD-B49E-0785FF9CFDDB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CB9A2C0-E860-4BCD-B49E-0785FF9CFDDB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>